<commit_message>
chore: update tables to match latest format
</commit_message>
<xml_diff>
--- a/GameData/EnemyData.xlsx
+++ b/GameData/EnemyData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t xml:space="preserve">namespace=TestGame.BattleSystem</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Fixed Item Drop</t>
   </si>
   <si>
+    <t xml:space="preserve">#active</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t xml:space="preserve">reward.count</t>
   </si>
   <si>
+    <t xml:space="preserve">bool</t>
+  </si>
+  <si>
     <t xml:space="preserve">int</t>
   </si>
   <si>
@@ -85,6 +91,15 @@
     <t xml:space="preserve">Reward</t>
   </si>
   <si>
+    <t xml:space="preserve">skip\n0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all\r\n1111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABC</t>
   </si>
   <si>
@@ -92,6 +107,21 @@
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5,8,14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5,8,15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5,8,16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5,8,17</t>
   </si>
 </sst>
 </file>
@@ -169,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +209,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,16 +237,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="15.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.28"/>
   </cols>
   <sheetData>
@@ -218,27 +255,27 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -268,61 +305,245 @@
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="G6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="n">
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>6003</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>6004</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1002</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>6005</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="J5" s="2" t="n">
-        <v>5</v>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>6006</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>6007</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add bool field in test table
</commit_message>
<xml_diff>
--- a/GameData/EnemyData.xlsx
+++ b/GameData/EnemyData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t xml:space="preserve">namespace=TestGame.BattleSystem</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isShow</t>
   </si>
   <si>
     <t xml:space="preserve">attack</t>
@@ -237,16 +240,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="15.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="15.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,19 +263,20 @@
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -308,241 +312,265 @@
       <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="H6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2" t="n">
         <v>6003</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="L6" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1001</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="H7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="2" t="n">
         <v>6004</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="L7" s="2" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1002</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2" t="n">
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="H8" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="n">
         <v>6005</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="L8" s="2" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1003</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="H9" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="2" t="n">
         <v>6006</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="L9" s="2" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1004</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="2" t="n">
+      <c r="E10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="H10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="2" t="n">
         <v>6007</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="L10" s="2" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>